<commit_message>
Actualización de horas. Cosas en proceso
</commit_message>
<xml_diff>
--- a/docs/gestion/AlbaAlmoril_Tareas.xlsx
+++ b/docs/gestion/AlbaAlmoril_Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\TFG\zenhabits-project\docs\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7480B3E-068E-48A6-9209-037321B098FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB5B1B-587C-4E82-9C39-B4229EDD1E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3288" yWindow="1620" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,19 +161,19 @@
     <t>TOTAL REAL</t>
   </si>
   <si>
-    <t>5 (ongoing)</t>
-  </si>
-  <si>
-    <t>1 (ongoing)</t>
-  </si>
-  <si>
     <t>*Es MUY posible que me den brotes y haya semanas que haga MUCHAS más horas u muchas MENOS</t>
   </si>
   <si>
-    <t>10 (ongoing)</t>
-  </si>
-  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>media (ongoing)</t>
+  </si>
+  <si>
+    <t>2 (ongoing)</t>
+  </si>
+  <si>
+    <t>12 (ongoing)</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,8 +1048,8 @@
       <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>44</v>
+      <c r="E5" s="1">
+        <v>15</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>14</v>
@@ -1068,8 +1068,8 @@
       <c r="D6" s="1">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
+      <c r="E6" s="1">
+        <v>7</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>36</v>
@@ -1089,7 +1089,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>37</v>
@@ -1108,7 +1108,9 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1125,7 +1127,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>20</v>
@@ -1145,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>22</v>
@@ -1182,7 +1184,9 @@
       <c r="D12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F12" s="12" t="s">
         <v>27</v>
       </c>
@@ -1249,12 +1253,12 @@
       </c>
       <c r="E17" s="19">
         <f>SUM(E2:E12)</f>
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>

</xml_diff>

<commit_message>
Update docs to latest main version
</commit_message>
<xml_diff>
--- a/docs/gestion/AlbaAlmoril_Tareas.xlsx
+++ b/docs/gestion/AlbaAlmoril_Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\TFG\zenhabits-project\docs\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAB5B1B-587C-4E82-9C39-B4229EDD1E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FAAE9-E11E-4D74-9F82-ACEAD28325D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3288" yWindow="1620" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Que sea fácil de seguir/utilizar</t>
   </si>
   <si>
-    <t>Crear presentación</t>
-  </si>
-  <si>
     <t>Presentación final del proyecto</t>
   </si>
   <si>
@@ -167,13 +164,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>media (ongoing)</t>
-  </si>
-  <si>
-    <t>2 (ongoing)</t>
-  </si>
-  <si>
-    <t>12 (ongoing)</t>
+    <t>Crear presentación y preparar defensa</t>
   </si>
 </sst>
 </file>
@@ -419,7 +410,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,7 +436,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -941,7 +931,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,7 +1001,7 @@
       <c r="E3" s="1">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1031,8 +1021,8 @@
       <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>38</v>
+      <c r="F4" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1051,7 +1041,7 @@
       <c r="E5" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1071,8 +1061,8 @@
       <c r="E6" s="1">
         <v>7</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>36</v>
+      <c r="F6" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1091,8 +1081,8 @@
       <c r="E7" s="1">
         <v>12</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>37</v>
+      <c r="F7" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1108,10 +1098,10 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="12"/>
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
@@ -1127,9 +1117,9 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1146,10 +1136,10 @@
       <c r="D10" s="1">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1166,8 +1156,10 @@
       <c r="D11" s="1">
         <v>7</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1176,7 +1168,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -1184,11 +1176,11 @@
       <c r="D12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>27</v>
+      <c r="E12" s="1">
+        <v>6</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1196,17 +1188,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1214,55 +1206,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="12" t="s">
+      <c r="D14" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F15" s="13" t="s">
+    <row r="16" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="D16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="19">
+      <c r="D17" s="18">
         <f>SUM(D2:D12)</f>
         <v>82</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="18">
         <f>SUM(E2:E12)</f>
-        <v>51</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="21"/>
+      <c r="B18" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>